<commit_message>
support import multi scenario
</commit_message>
<xml_diff>
--- a/Logiz.Radar/bin/Release/netcoreapp2.2/publish/wwwroot/template/logiz.radar.test-case.xlsx
+++ b/Logiz.Radar/bin/Release/netcoreapp2.2/publish/wwwroot/template/logiz.radar.test-case.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Note" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCase!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCase!$A$1:$Q$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>TestCaseName (*)</t>
   </si>
@@ -46,9 +46,6 @@
     <t>ActualResult</t>
   </si>
   <si>
-    <t xml:space="preserve">TestVariantName (*) </t>
-  </si>
-  <si>
     <t>System Validation (Do not fill-in)</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
     <t>Template version:</t>
   </si>
   <si>
-    <t>v1.0.0.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Updated by: </t>
   </si>
   <si>
@@ -86,6 +80,33 @@
   </si>
   <si>
     <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>CreatedBy</t>
+  </si>
+  <si>
+    <t>CreatedDateTime</t>
+  </si>
+  <si>
+    <t>ScenarioName</t>
+  </si>
+  <si>
+    <t>HasAttachment</t>
+  </si>
+  <si>
+    <t>UpdatedBy</t>
+  </si>
+  <si>
+    <t>UpdatedDateTime</t>
+  </si>
+  <si>
+    <t>v1.1.0.0</t>
+  </si>
+  <si>
+    <t>ScenarioID (*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VariantName (*) </t>
   </si>
 </sst>
 </file>
@@ -96,7 +117,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,14 +129,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,8 +148,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +174,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -161,9 +195,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -180,13 +214,19 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -470,32 +510,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="13.6328125" style="2"/>
-    <col min="14" max="14" width="13.6328125" style="10"/>
-    <col min="15" max="15" width="13.6328125" style="2"/>
-    <col min="16" max="16" width="18.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="13.6328125" style="2"/>
+    <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.54296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="13.6328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -519,19 +562,40 @@
         <v>5</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
+      <c r="P1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:Q1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>"Passed, Failed, Open, Pending, Hold, Canceled"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -553,53 +617,53 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8">
-        <v>43731</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="7">
+        <v>43745</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add column Note for TestCase
</commit_message>
<xml_diff>
--- a/Logiz.Radar/bin/Release/netcoreapp2.2/publish/wwwroot/template/logiz.radar.test-case.xlsx
+++ b/Logiz.Radar/bin/Release/netcoreapp2.2/publish/wwwroot/template/logiz.radar.test-case.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Note" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCase!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestCase!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>TestCaseName (*)</t>
   </si>
@@ -100,12 +100,15 @@
     <t xml:space="preserve">VariantName (*) </t>
   </si>
   <si>
-    <t>- Do not change ordinal of columns in the left of column K. 
+    <t>Note</t>
+  </si>
+  <si>
+    <t>v1.3.1.0</t>
+  </si>
+  <si>
+    <t>- Do not change ordinal of columns in the left of column System Validation. 
 - Can change name of any columns.
-- Can add or remove columns in the right of column K.</t>
-  </si>
-  <si>
-    <t>v1.3.0.0</t>
+- Can add or remove columns in the right of column System Validation.</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -519,21 +522,22 @@
   <cols>
     <col min="1" max="5" width="30.453125" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.90625" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="13.6328125" style="2"/>
+    <col min="7" max="7" width="30.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.90625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="13.6328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -553,46 +557,49 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1"/>
+  <autoFilter ref="A1:R1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Passed, Failed, Fixed, Open, Pending, Hold, Canceled"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -609,7 +616,7 @@
   <cols>
     <col min="1" max="1" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7265625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -633,7 +640,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="6">
-        <v>43749</v>
+        <v>43753</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
@@ -641,10 +648,10 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>